<commit_message>
mod z score excel file
</commit_message>
<xml_diff>
--- a/modified_zscore.xlsx
+++ b/modified_zscore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATHS AND STATISTICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC130E6-DD3A-411C-8AD4-F75A270141D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99173F14-4565-4E51-AACA-0D464A6BE802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42676532-4AE6-44FF-965A-C610EE8DB39A}">
   <dimension ref="A6:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>